<commit_message>
maj de la BOM
</commit_message>
<xml_diff>
--- a/Afficheur rapport/rapport_bom.xlsx
+++ b/Afficheur rapport/rapport_bom.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\STUF2019\EL - Electrical\Autre\Tableau de bord\Carte élecs\Afficheur rapport\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EPSA\Dashboard_display\Afficheur rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2533967A-56FE-4A32-8BCF-9CC4E7B78526}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAEA564-0F9F-4367-ADC1-2D93FE6708C9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rapport_bom" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -698,7 +698,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -717,27 +717,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1055,11 +1034,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="F10:G10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,7 +1199,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$L$1:$L$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>